<commit_message>
fixed monte carlo function which had the final results transposed after some double checking
</commit_message>
<xml_diff>
--- a/monte_carlo_simulation_results.xlsx
+++ b/monte_carlo_simulation_results.xlsx
@@ -408,16 +408,16 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.604185</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <v>0.202615</v>
+        <v>0</v>
       </c>
       <c r="D2">
-        <v>0.121285</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>0.07191500000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -425,16 +425,16 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.236123</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>0.404708</v>
+        <v>0.24931</v>
       </c>
       <c r="D3">
-        <v>0.301282</v>
+        <v>0.75069</v>
       </c>
       <c r="E3">
-        <v>0.057887</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -442,16 +442,16 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.019264</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <v>0.087162</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>0.179536</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>0.714038</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -459,16 +459,16 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.140428</v>
+        <v>0</v>
       </c>
       <c r="C5">
-        <v>0.305515</v>
+        <v>0.75069</v>
       </c>
       <c r="D5">
-        <v>0.397897</v>
+        <v>0.24931</v>
       </c>
       <c r="E5">
-        <v>0.15616</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
I updated the cycle determinening function. Now it can cut off the ends if there is no current at the end to the last current point and those bpoints are more than an hour apart
</commit_message>
<xml_diff>
--- a/monte_carlo_simulation_results.xlsx
+++ b/monte_carlo_simulation_results.xlsx
@@ -408,16 +408,16 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>0.60409275</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>0.20266954</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>0.12120013</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>0.07203758</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -425,16 +425,16 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>0.23597553</v>
       </c>
       <c r="C3">
-        <v>0.24931</v>
+        <v>0.40452926</v>
       </c>
       <c r="D3">
-        <v>0.75069</v>
+        <v>0.30179174</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>0.05770347</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -442,16 +442,16 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>0.01916627</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>0.0871682</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>0.17918482</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>0.71448071</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -459,16 +459,16 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>0.14076545</v>
       </c>
       <c r="C5">
-        <v>0.75069</v>
+        <v>0.305633</v>
       </c>
       <c r="D5">
-        <v>0.24931</v>
+        <v>0.39782331</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>0.15577824</v>
       </c>
     </row>
   </sheetData>

</xml_diff>